<commit_message>
update Excel and graph
</commit_message>
<xml_diff>
--- a/QuickSortTimeData.xlsx
+++ b/QuickSortTimeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bni/Documents/CS/HanSolo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A63C457-0C2E-3945-8A36-1F6C60F8B953}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8978B66E-D5B9-5F43-95B7-74B6A42CD3BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{C8EF85DF-41AF-3545-A990-5D5338FAEF36}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{C8EF85DF-41AF-3545-A990-5D5338FAEF36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$R$3:$R$202</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$R$3:$R$202</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$3:$A$202</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$R$3:$R$202</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -224,6 +226,615 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$202</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2350</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2450</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2650</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2850</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2950</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3050</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3150</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3350</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3550</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3650</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4150</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4350</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4450</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4550</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4650</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4850</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4950</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>5050</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5150</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>5350</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>5450</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>5550</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>5650</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5700</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>5750</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>5850</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5950</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>6050</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>6100</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>6150</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>6250</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>6300</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>6350</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>6450</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>6550</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>6650</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>6750</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>6850</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>6900</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>6950</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>7050</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>7100</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>7150</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>7200</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>7250</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>7350</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>7400</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>7450</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>7550</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>7600</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>7650</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>7750</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>7850</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>7900</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>7950</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>8050</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>8150</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>8200</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>8250</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>8300</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>8350</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>8450</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>8550</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>8600</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>8650</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>8700</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>8750</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>8850</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>8900</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>8950</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>9050</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>9100</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>9150</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>9250</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>9300</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>9350</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>9400</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>9450</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>9550</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>9650</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>9700</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>9750</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>9800</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>9850</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>9900</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>9950</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$R$3:$R$202</c:f>
@@ -1687,8 +2298,8 @@
       <xdr:rowOff>19542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>688555</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>168313</xdr:rowOff>
     </xdr:to>
@@ -2017,8 +2628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47366DF4-626B-6D44-BE51-144B7F87B80D}">
   <dimension ref="A1:R203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="O5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H233" sqref="H228:J233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>